<commit_message>
Combined storage plot at end of PowellMead
</commit_message>
<xml_diff>
--- a/MeadPowellPlots/MeadLevel.xlsx
+++ b/MeadPowellPlots/MeadLevel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\Walton\CODocs\MeadPowellPlots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\MeadPowellPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883C0B5E-A830-415D-ACFA-9673DA1FEC25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MeadLevelEndOfMonth" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Year</t>
   </si>
@@ -64,11 +65,14 @@
   <si>
     <t>DEC</t>
   </si>
+  <si>
+    <t>2019</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,16 +440,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="P65" sqref="P65"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:M88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +490,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1935</v>
       </c>
@@ -525,7 +529,7 @@
         <v>908.4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1936</v>
       </c>
@@ -566,7 +570,7 @@
         <v>1023.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1937</v>
       </c>
@@ -607,7 +611,7 @@
         <v>1095.75</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1938</v>
       </c>
@@ -648,7 +652,7 @@
         <v>1168.6500000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1939</v>
       </c>
@@ -689,7 +693,7 @@
         <v>1169.95</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1940</v>
       </c>
@@ -730,7 +734,7 @@
         <v>1168.05</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1941</v>
       </c>
@@ -771,7 +775,7 @@
         <v>1195.8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1942</v>
       </c>
@@ -812,7 +816,7 @@
         <v>1188.4000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1943</v>
       </c>
@@ -853,7 +857,7 @@
         <v>1178.3499999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1944</v>
       </c>
@@ -894,7 +898,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1945</v>
       </c>
@@ -935,7 +939,7 @@
         <v>1163.3499999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1946</v>
       </c>
@@ -976,7 +980,7 @@
         <v>1148.55</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1947</v>
       </c>
@@ -1017,7 +1021,7 @@
         <v>1170.58</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1948</v>
       </c>
@@ -1058,7 +1062,7 @@
         <v>1164.8499999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1949</v>
       </c>
@@ -1099,7 +1103,7 @@
         <v>1170.06</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>1950</v>
       </c>
@@ -1140,7 +1144,7 @@
         <v>1156.6199999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1951</v>
       </c>
@@ -1181,7 +1185,7 @@
         <v>1153.1199999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1952</v>
       </c>
@@ -1222,7 +1226,7 @@
         <v>1169.0999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1953</v>
       </c>
@@ -1263,7 +1267,7 @@
         <v>1145.78</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1954</v>
       </c>
@@ -1304,7 +1308,7 @@
         <v>1105.4000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1955</v>
       </c>
@@ -1345,7 +1349,7 @@
         <v>1090.99</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1956</v>
       </c>
@@ -1386,7 +1390,7 @@
         <v>1097.02</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1957</v>
       </c>
@@ -1427,7 +1431,7 @@
         <v>1177.3900000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>1958</v>
       </c>
@@ -1468,7 +1472,7 @@
         <v>1185.8499999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>1959</v>
       </c>
@@ -1509,7 +1513,7 @@
         <v>1167.28</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>1960</v>
       </c>
@@ -1550,7 +1554,7 @@
         <v>1165.1199999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>1961</v>
       </c>
@@ -1591,7 +1595,7 @@
         <v>1154.6400000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>1962</v>
       </c>
@@ -1632,7 +1636,7 @@
         <v>1193.1199999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>1963</v>
       </c>
@@ -1673,7 +1677,7 @@
         <v>1136.93</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>1964</v>
       </c>
@@ -1714,7 +1718,7 @@
         <v>1088.1400000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>1965</v>
       </c>
@@ -1755,7 +1759,7 @@
         <v>1129.74</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>1966</v>
       </c>
@@ -1796,7 +1800,7 @@
         <v>1132.05</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>1967</v>
       </c>
@@ -1837,7 +1841,7 @@
         <v>1129.8399999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>1968</v>
       </c>
@@ -1878,7 +1882,7 @@
         <v>1139.6500000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>1969</v>
       </c>
@@ -1919,7 +1923,7 @@
         <v>1152.5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>1970</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>1152.95</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>1971</v>
       </c>
@@ -2001,7 +2005,7 @@
         <v>1160.1300000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>1972</v>
       </c>
@@ -2042,7 +2046,7 @@
         <v>1168.3499999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>1973</v>
       </c>
@@ -2083,7 +2087,7 @@
         <v>1176.92</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>1974</v>
       </c>
@@ -2124,7 +2128,7 @@
         <v>1176.8</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>1975</v>
       </c>
@@ -2165,7 +2169,7 @@
         <v>1179.6300000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>1976</v>
       </c>
@@ -2206,7 +2210,7 @@
         <v>1187.8699999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1977</v>
       </c>
@@ -2247,7 +2251,7 @@
         <v>1180.82</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>1978</v>
       </c>
@@ -2288,7 +2292,7 @@
         <v>1193.31</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>1979</v>
       </c>
@@ -2329,7 +2333,7 @@
         <v>1197.97</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>1980</v>
       </c>
@@ -2370,7 +2374,7 @@
         <v>1202.8800000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>1981</v>
       </c>
@@ -2411,7 +2415,7 @@
         <v>1198.28</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>1982</v>
       </c>
@@ -2452,7 +2456,7 @@
         <v>1208.3699999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>1983</v>
       </c>
@@ -2493,7 +2497,7 @@
         <v>1212.33</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>1984</v>
       </c>
@@ -2534,7 +2538,7 @@
         <v>1207.9000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>1985</v>
       </c>
@@ -2575,7 +2579,7 @@
         <v>1205.49</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>1986</v>
       </c>
@@ -2616,7 +2620,7 @@
         <v>1210.3900000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>1987</v>
       </c>
@@ -2657,7 +2661,7 @@
         <v>1211.03</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>1988</v>
       </c>
@@ -2698,7 +2702,7 @@
         <v>1199.75</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>1989</v>
       </c>
@@ -2739,7 +2743,7 @@
         <v>1189.8</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>1990</v>
       </c>
@@ -2780,7 +2784,7 @@
         <v>1177.8900000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>1991</v>
       </c>
@@ -2821,7 +2825,7 @@
         <v>1173.44</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>1992</v>
       </c>
@@ -2862,7 +2866,7 @@
         <v>1176.8599999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>1993</v>
       </c>
@@ -2903,7 +2907,7 @@
         <v>1188.75</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>1994</v>
       </c>
@@ -2944,7 +2948,7 @@
         <v>1176.55</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>1995</v>
       </c>
@@ -2985,7 +2989,7 @@
         <v>1190.92</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>1996</v>
       </c>
@@ -3026,7 +3030,7 @@
         <v>1194.3800000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>1997</v>
       </c>
@@ -3067,7 +3071,7 @@
         <v>1214.6400000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>1998</v>
       </c>
@@ -3108,7 +3112,7 @@
         <v>1212.53</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>1999</v>
       </c>
@@ -3149,7 +3153,7 @@
         <v>1213.94</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>2000</v>
       </c>
@@ -3190,7 +3194,7 @@
         <v>1196.1199999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>2001</v>
       </c>
@@ -3231,7 +3235,7 @@
         <v>1177.3699999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>2002</v>
       </c>
@@ -3272,7 +3276,7 @@
         <v>1152.1300000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>2003</v>
       </c>
@@ -3313,7 +3317,7 @@
         <v>1139.1199999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>2004</v>
       </c>
@@ -3354,7 +3358,7 @@
         <v>1130.01</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>2005</v>
       </c>
@@ -3395,7 +3399,7 @@
         <v>1137.52</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>2006</v>
       </c>
@@ -3436,7 +3440,7 @@
         <v>1128.1199999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>2007</v>
       </c>
@@ -3477,7 +3481,7 @@
         <v>1114.81</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>2008</v>
       </c>
@@ -3518,7 +3522,7 @@
         <v>1110.97</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>2009</v>
       </c>
@@ -3559,7 +3563,7 @@
         <v>1096.3</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>2010</v>
       </c>
@@ -3600,7 +3604,7 @@
         <v>1086.3</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>2011</v>
       </c>
@@ -3641,7 +3645,7 @@
         <v>1132.83</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>2012</v>
       </c>
@@ -3682,7 +3686,7 @@
         <v>1120.3599999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>2013</v>
       </c>
@@ -3723,7 +3727,7 @@
         <v>1106.73</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>2014</v>
       </c>
@@ -3764,7 +3768,7 @@
         <v>1087.79</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>2015</v>
       </c>
@@ -3805,7 +3809,7 @@
         <v>1080.9100000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>2016</v>
       </c>
@@ -3846,7 +3850,7 @@
         <v>1080.82</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>2017</v>
       </c>
@@ -3887,7 +3891,7 @@
         <v>1082.52</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>2018</v>
       </c>
@@ -3928,24 +3932,114 @@
         <v>1081.46</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="3">
-        <v>2019</v>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B86" s="4">
         <v>1085.75</v>
       </c>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
-      <c r="L86" s="5"/>
-      <c r="M86" s="6"/>
+      <c r="C86" s="4">
+        <v>1087.97</v>
+      </c>
+      <c r="D86" s="4">
+        <v>1090.24</v>
+      </c>
+      <c r="E86" s="4">
+        <v>1088.95</v>
+      </c>
+      <c r="F86" s="4">
+        <v>1086.48</v>
+      </c>
+      <c r="G86" s="4">
+        <v>1084.71</v>
+      </c>
+      <c r="H86" s="4">
+        <v>1082.82</v>
+      </c>
+      <c r="I86" s="4">
+        <v>1083.45</v>
+      </c>
+      <c r="J86" s="4">
+        <v>1083</v>
+      </c>
+      <c r="K86" s="4">
+        <v>1082.6099999999999</v>
+      </c>
+      <c r="L86" s="4">
+        <v>1083.8499999999999</v>
+      </c>
+      <c r="M86" s="4">
+        <v>1090.49</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A87" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B87" s="4">
+        <v>1094.68</v>
+      </c>
+      <c r="C87" s="4">
+        <v>1096.27</v>
+      </c>
+      <c r="D87" s="4">
+        <v>1098.5899999999999</v>
+      </c>
+      <c r="E87" s="4">
+        <v>1096.3900000000001</v>
+      </c>
+      <c r="F87" s="4">
+        <v>1091.32</v>
+      </c>
+      <c r="G87" s="4">
+        <v>1087.07</v>
+      </c>
+      <c r="H87" s="4">
+        <v>1084.6300000000001</v>
+      </c>
+      <c r="I87" s="4">
+        <v>1084.04</v>
+      </c>
+      <c r="J87" s="4">
+        <v>1083.21</v>
+      </c>
+      <c r="K87" s="4">
+        <v>1081.8800000000001</v>
+      </c>
+      <c r="L87" s="4">
+        <v>1081.07</v>
+      </c>
+      <c r="M87" s="4">
+        <v>1083.72</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A88" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B88" s="4">
+        <v>1085.95</v>
+      </c>
+      <c r="C88" s="4">
+        <v>1087.26</v>
+      </c>
+      <c r="D88" s="4">
+        <v>1084.3900000000001</v>
+      </c>
+      <c r="E88" s="4">
+        <v>1079.3</v>
+      </c>
+      <c r="F88" s="4">
+        <v>1073.5</v>
+      </c>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>